<commit_message>
cars slowing and accelerating within safe limits~! Would like to see the tailing distance reigned in though, seems overly safe...
</commit_message>
<xml_diff>
--- a/ASPNETCore-SignalR-Angular-TypeScript/App/Game/SpeedCalculations.xlsx
+++ b/ASPNETCore-SignalR-Angular-TypeScript/App/Game/SpeedCalculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\games\HazardHighway\ASPNETCore-SignalR-Angular-TypeScript\App\Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154ABAA6-A410-4C9F-85AB-3A59A1622DDE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5624DC3C-1A67-493C-90D6-4212BB227CBF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="8160" xr2:uid="{6110ACBD-490E-4EE7-AB26-B94330B23FB7}"/>
   </bookViews>
@@ -527,7 +527,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AO8" sqref="AO8"/>
+      <selection pane="topRight" activeCell="AU11" sqref="AU11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -539,7 +539,8 @@
     <col min="10" max="10" width="33.734375" customWidth="1"/>
     <col min="11" max="27" width="3.68359375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="33.5234375" customWidth="1"/>
-    <col min="30" max="46" width="3.68359375" bestFit="1" customWidth="1"/>
+    <col min="30" max="36" width="3.68359375" bestFit="1" customWidth="1"/>
+    <col min="37" max="46" width="4.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:46" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1374,49 +1375,19 @@
         <v>276</v>
       </c>
       <c r="AF9">
-        <v>310</v>
+        <v>286</v>
       </c>
       <c r="AG9">
-        <v>318</v>
+        <v>294</v>
       </c>
       <c r="AH9">
-        <v>324</v>
+        <v>300</v>
       </c>
       <c r="AI9">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="AJ9">
-        <v>330</v>
-      </c>
-      <c r="AK9">
-        <v>330</v>
-      </c>
-      <c r="AL9">
-        <v>330</v>
-      </c>
-      <c r="AM9">
-        <v>330</v>
-      </c>
-      <c r="AN9">
-        <v>330</v>
-      </c>
-      <c r="AO9">
-        <v>330</v>
-      </c>
-      <c r="AP9">
-        <v>330</v>
-      </c>
-      <c r="AQ9">
-        <v>330</v>
-      </c>
-      <c r="AR9">
-        <v>330</v>
-      </c>
-      <c r="AS9">
-        <v>330</v>
-      </c>
-      <c r="AT9">
-        <v>330</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.55000000000000004">
@@ -1562,63 +1533,63 @@
       </c>
       <c r="AF11" s="3">
         <f>SUM(AF9-AF18)</f>
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="AG11" s="3">
         <f>SUM(AG9-AG18)</f>
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="AH11" s="3">
         <f>SUM(AH9-AH18)</f>
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="AI11" s="4">
         <f>SUM(AI9-AI18)</f>
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="AJ11" s="4">
         <f>SUM(AJ9-AJ18)</f>
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="AK11" s="4">
         <f>SUM(AK9-AK18)</f>
-        <v>33</v>
+        <v>-297</v>
       </c>
       <c r="AL11">
         <f t="shared" ref="AL11:AT11" si="5">SUM(AL9-AL18)</f>
-        <v>29</v>
+        <v>-301</v>
       </c>
       <c r="AM11" s="4">
         <f t="shared" si="5"/>
-        <v>25</v>
+        <v>-305</v>
       </c>
       <c r="AN11" s="3">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>-309</v>
       </c>
       <c r="AO11">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>-317</v>
       </c>
       <c r="AP11">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>-319</v>
       </c>
       <c r="AQ11">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>-321</v>
       </c>
       <c r="AR11">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>-323</v>
       </c>
       <c r="AS11">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>-325</v>
       </c>
       <c r="AT11">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>-327</v>
       </c>
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.55000000000000004">

</xml_diff>